<commit_message>
Setting up frontend backend project
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="93">
   <si>
     <t>ECommerce site</t>
   </si>
@@ -271,21 +271,212 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>Optional information,intrest of user</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Foreign key Relation With Shipping Information table</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Foreign key Relation With Billing Information table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Created Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Date and time when system has created a record.</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Required information , Default set to true</t>
+  </si>
+  <si>
+    <t>Table :- Category</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CategoryName</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Required Information</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Table :- Sub Category</t>
+  </si>
+  <si>
+    <t>Category Id</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation With Category table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubCategoryName</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Table :- Product</t>
+  </si>
+  <si>
+    <t>SubCategory Id</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation With SubCategory table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ProductName</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Optional information</t>
   </si>
   <si>
-    <t>Shipping Address</t>
-  </si>
-  <si>
-    <t>Foreign key Relation With Shipping Information table</t>
-  </si>
-  <si>
-    <t>Billing Address</t>
-  </si>
-  <si>
-    <t>Foreign key Relation With Billing Information table</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -294,10 +485,138 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Created Date</t>
-    </r>
-    <r>
-      <rPr>
+      <t>Image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Required information,Small = 0 ,Medium =1,Large=2</t>
+  </si>
+  <si>
+    <t>Table :- Order</t>
+  </si>
+  <si>
+    <t>Product id</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation With Product table</t>
+  </si>
+  <si>
+    <t>Userid</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation With User table</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>Status Of Order</t>
+  </si>
+  <si>
+    <t>Modified Date</t>
+  </si>
+  <si>
+    <t>Date and time when Status has been modified.</t>
+  </si>
+  <si>
+    <t>Table :-  ContactUs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -308,24 +627,6 @@
     </r>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>Date and time when system has created a record.</t>
-  </si>
-  <si>
-    <t>IsActive</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>Required information , Default set to true</t>
-  </si>
-  <si>
-    <t>Table :- Category</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -334,12 +635,83 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Id</t>
+      <t>EmailID</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Subject</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Comment</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Table :-  Shipping Information</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="5"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
@@ -349,9 +721,6 @@
     </r>
   </si>
   <si>
-    <t>PRIMARY KEY</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -360,12 +729,96 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CategoryName</t>
+      <t>Street</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>City</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>State</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Foreign Key Relation with State table</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation with Country table</t>
+  </si>
+  <si>
+    <t>Table :-  Billing Information</t>
+  </si>
+  <si>
+    <t>Table :- Country</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CountryName</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
         <color theme="5"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
@@ -383,7 +836,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Description</t>
+      <t>Countrycode</t>
     </r>
     <r>
       <rPr>
@@ -398,22 +851,7 @@
     </r>
   </si>
   <si>
-    <t>Required Information</t>
-  </si>
-  <si>
-    <t>CreatedDate</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Table :- Sub Category</t>
-  </si>
-  <si>
-    <t>Category Id</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation With Category table</t>
+    <t>Table :- State</t>
   </si>
   <si>
     <r>
@@ -424,7 +862,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SubCategoryName</t>
+      <t>Countryid</t>
     </r>
     <r>
       <rPr>
@@ -439,354 +877,7 @@
     </r>
   </si>
   <si>
-    <t>Table :- Product</t>
-  </si>
-  <si>
-    <t>SubCategory Id</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation With SubCategory table</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ProductName</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Required information,Small = 0 ,Medium =1,Large=2</t>
-  </si>
-  <si>
-    <t>Table :- Order</t>
-  </si>
-  <si>
-    <t>Product id</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation With Product table</t>
-  </si>
-  <si>
-    <t>Userid</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation With User table</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Varchar</t>
-  </si>
-  <si>
-    <t>Status Of Order</t>
-  </si>
-  <si>
-    <t>Modified Date</t>
-  </si>
-  <si>
-    <t>Date and time when Status has been modified.</t>
-  </si>
-  <si>
-    <t>Table :-  ContactUs</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EmailID</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Subject</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Comment</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Table :-  Shipping Information</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UserId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Street</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>City</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>State</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Table :-  Billing Information</t>
-  </si>
-  <si>
-    <t>Table :- Country</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CountryName</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Countrycode</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Table :- State</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Countryid</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
+    <t>Foreignkey Relation With Country table</t>
   </si>
   <si>
     <r>
@@ -817,9 +908,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -871,13 +962,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,7 +972,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -911,6 +1002,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -918,11 +1017,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -949,23 +1061,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -973,21 +1079,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1023,16 +1114,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="5"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1071,7 +1162,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1089,13 +1198,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1107,7 +1216,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,7 +1234,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,7 +1270,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,13 +1294,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1161,67 +1306,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1233,13 +1330,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1321,6 +1412,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1341,44 +1456,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1391,127 +1482,127 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1879,8 +1970,8 @@
   <sheetPr/>
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2116,7 +2207,7 @@
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>34</v>
@@ -2473,7 +2564,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="12" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>12</v>
@@ -2485,12 +2576,12 @@
         <v>45</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>12</v>
@@ -2507,7 +2598,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>12</v>
@@ -2524,7 +2615,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>8</v>
@@ -2541,7 +2632,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>8</v>
@@ -2551,7 +2642,7 @@
         <v>9</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2586,7 +2677,7 @@
     </row>
     <row r="58" ht="18.75" spans="1:5">
       <c r="A58" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -2634,7 +2725,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>8</v>
@@ -2644,12 +2735,12 @@
         <v>23</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>8</v>
@@ -2659,12 +2750,12 @@
         <v>23</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>8</v>
@@ -2679,10 +2770,10 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C65" s="13">
         <v>50</v>
@@ -2691,7 +2782,7 @@
         <v>26</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2711,7 +2802,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>33</v>
@@ -2721,7 +2812,7 @@
         <v>23</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2741,7 +2832,7 @@
     </row>
     <row r="71" ht="18.75" spans="1:5">
       <c r="A71" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -2774,7 +2865,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>8</v>
@@ -2789,7 +2880,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>12</v>
@@ -2806,7 +2897,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>12</v>
@@ -2823,7 +2914,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>12</v>
@@ -2870,7 +2961,7 @@
     </row>
     <row r="82" ht="18.75" spans="1:5">
       <c r="A82" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -2903,7 +2994,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>8</v>
@@ -2918,7 +3009,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>8</v>
@@ -2928,12 +3019,12 @@
         <v>23</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>12</v>
@@ -2950,14 +3041,12 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="13">
-        <v>50</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C88" s="13"/>
       <c r="D88" s="6" t="s">
         <v>9</v>
       </c>
@@ -2967,24 +3056,22 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C89" s="13">
-        <v>250</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C89" s="13"/>
       <c r="D89" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>12</v>
@@ -2996,7 +3083,7 @@
         <v>23</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -3031,7 +3118,7 @@
     </row>
     <row r="94" ht="18.75" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -3064,7 +3151,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>8</v>
@@ -3079,7 +3166,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>8</v>
@@ -3089,12 +3176,12 @@
         <v>23</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>12</v>
@@ -3111,7 +3198,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>12</v>
@@ -3128,36 +3215,32 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C101" s="13">
-        <v>250</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C101" s="13"/>
       <c r="D101" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C102" s="13">
-        <v>250</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C102" s="13"/>
       <c r="D102" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -3192,7 +3275,7 @@
     </row>
     <row r="107" ht="18.75" spans="1:5">
       <c r="A107" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -3240,7 +3323,7 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>12</v>
@@ -3257,7 +3340,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>12</v>
@@ -3304,7 +3387,7 @@
     </row>
     <row r="117" ht="18.75" spans="1:5">
       <c r="A117" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -3352,24 +3435,22 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C121" s="13">
-        <v>50</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C121" s="13"/>
       <c r="D121" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="12" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
change in excel file
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -250,6 +250,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Mobile no</t>
     </r>
     <r>
@@ -321,6 +328,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Modified Date</t>
     </r>
     <r>
@@ -530,6 +544,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Color id</t>
     </r>
     <r>
@@ -570,6 +591,66 @@
   </si>
   <si>
     <r>
+      <t>Size Id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Foreign Key Relation With Size table</t>
+  </si>
+  <si>
+    <t>SKU ID*</t>
+  </si>
+  <si>
+    <t>Table :- Order</t>
+  </si>
+  <si>
+    <t>Product id</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation With Product table</t>
+  </si>
+  <si>
+    <t>Userid</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation With User table</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Tax Amount</t>
+  </si>
+  <si>
+    <t>Delievery Status</t>
+  </si>
+  <si>
+    <t>delivered=4,out for delievery = 3,shipped=2,packed=1,ordered=0,</t>
+  </si>
+  <si>
+    <t>Modified Date</t>
+  </si>
+  <si>
+    <t>Date and time when Status has been modified.</t>
+  </si>
+  <si>
+    <t>Table :-  ContactUs</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -577,7 +658,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Size</t>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name</t>
     </r>
     <r>
       <rPr>
@@ -591,51 +695,6 @@
     </r>
   </si>
   <si>
-    <t>Foreign Key Relation With Size table</t>
-  </si>
-  <si>
-    <t>SKU ID*</t>
-  </si>
-  <si>
-    <t>Table :- Order</t>
-  </si>
-  <si>
-    <t>Product id</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation With Product table</t>
-  </si>
-  <si>
-    <t>Userid</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation With User table</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
-  </si>
-  <si>
-    <t>Tax Amount</t>
-  </si>
-  <si>
-    <t>Delievery Status</t>
-  </si>
-  <si>
-    <t>delivered=4,out for delievery = 3,shipped=2,packed=1,ordered=0,</t>
-  </si>
-  <si>
-    <t>Modified Date</t>
-  </si>
-  <si>
-    <t>Date and time when Status has been modified.</t>
-  </si>
-  <si>
-    <t>Table :-  ContactUs</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -644,7 +703,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ID</t>
+      <t>EmailID</t>
     </r>
     <r>
       <rPr>
@@ -660,10 +719,251 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Subject</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Comment</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Table :-  Shipping Information</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Street</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>City</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Foreign Key Relation with City table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>State</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Foreign Key Relation with State table</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Foreign Key Relation with Country table</t>
+  </si>
+  <si>
+    <t>Table :-  Billing Information</t>
+  </si>
+  <si>
+    <t>Table :- Country</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CountryName</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Countrycode</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Table :- State</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Countryid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Foreignkey Relation With Country table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Name</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="5"/>
         <rFont val="Calibri"/>
@@ -674,6 +974,9 @@
     </r>
   </si>
   <si>
+    <t>Table :- City</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -682,13 +985,13 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>EmailID</t>
+      <t>Stateid</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="5"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -697,6 +1000,12 @@
     </r>
   </si>
   <si>
+    <t>Foreignkey Relation With State table</t>
+  </si>
+  <si>
+    <t>Table :- Color</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -705,13 +1014,12 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Subject</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t>ColorCode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -720,6 +1028,15 @@
     </r>
   </si>
   <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>Table :- Size</t>
+  </si>
+  <si>
+    <t>Table :- Tax</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -728,281 +1045,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Comment</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Table :-  Shipping Information</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UserId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Street</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>City</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Foreign Key Relation with City table</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>State</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Foreign Key Relation with State table</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Foreign Key Relation with Country table</t>
-  </si>
-  <si>
-    <t>Table :-  Billing Information</t>
-  </si>
-  <si>
-    <t>Table :- Country</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CountryName</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Countrycode</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Table :- State</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Countryid</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Foreignkey Relation With Country table</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Name</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Table :- City</t>
-  </si>
-  <si>
-    <r>
-      <t>Stateid</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Foreignkey Relation With State table</t>
-  </si>
-  <si>
-    <t>Table :- Color</t>
-  </si>
-  <si>
-    <r>
-      <t>ColorCode</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Varchar</t>
-  </si>
-  <si>
-    <t>Table :- Size</t>
-  </si>
-  <si>
-    <t>Table :- Tax</t>
-  </si>
-  <si>
-    <r>
       <t>Country Id</t>
     </r>
     <r>
@@ -1032,9 +1074,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1079,9 +1121,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1094,31 +1142,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1140,21 +1174,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1170,6 +1189,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1178,8 +1205,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1193,7 +1237,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1201,21 +1245,19 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1286,31 +1328,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,7 +1376,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1346,43 +1484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1395,66 +1497,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1483,6 +1525,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1498,15 +1549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1518,39 +1560,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1572,6 +1581,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1580,12 +1598,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1603,130 +1645,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2097,8 +2139,8 @@
   <sheetPr/>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
complete till category page
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -591,6 +591,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Size Id</t>
     </r>
     <r>
@@ -1074,9 +1081,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1122,6 +1129,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1129,24 +1143,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1174,6 +1181,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1189,27 +1212,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1224,6 +1231,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1246,13 +1260,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1328,7 +1335,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1340,115 +1455,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1466,13 +1479,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1485,18 +1504,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1525,11 +1532,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1549,6 +1562,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1560,21 +1582,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1627,15 +1634,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1648,131 +1655,131 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1816,6 +1823,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2139,8 +2149,8 @@
   <sheetPr/>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2925,7 +2935,7 @@
       <c r="B59" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="15">
         <v>2</v>
       </c>
       <c r="D59" s="7" t="s">

</xml_diff>